<commit_message>
collection of all 'flags & factors' corresponding to delta customers
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/Excel worksheets/Flags.xlsx
+++ b/src/main/resources/Data/Excel worksheets/Flags.xlsx
@@ -594,7 +594,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1288,7 +1288,7 @@
         <v>59</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>12</v>
@@ -1297,7 +1297,7 @@
         <v>13</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>